<commit_message>
Update login and cart test cases
</commit_message>
<xml_diff>
--- a/testing-docs/bug-reports/Test_Register.xlsx
+++ b/testing-docs/bug-reports/Test_Register.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8130" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Test ScenarioS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -216,6 +217,81 @@
   </si>
   <si>
     <t>Validation message is displayed</t>
+  </si>
+  <si>
+    <t>Scenario ID</t>
+  </si>
+  <si>
+    <t>Scenario Name</t>
+  </si>
+  <si>
+    <t>Scenario Description</t>
+  </si>
+  <si>
+    <t>Related Test Case</t>
+  </si>
+  <si>
+    <t>TS_REG_01</t>
+  </si>
+  <si>
+    <t>TS_REG_02</t>
+  </si>
+  <si>
+    <t>TS_REG_03</t>
+  </si>
+  <si>
+    <t>TS_REG_04</t>
+  </si>
+  <si>
+    <t>TS_REG_05</t>
+  </si>
+  <si>
+    <t>TS_REG_06</t>
+  </si>
+  <si>
+    <t>TS_REG_07</t>
+  </si>
+  <si>
+    <t>Register with empty required 
+fields</t>
+  </si>
+  <si>
+    <t>Register with invalid email 
+format</t>
+  </si>
+  <si>
+    <t>Register with invalid password</t>
+  </si>
+  <si>
+    <t>Register with invalid name input</t>
+  </si>
+  <si>
+    <t>User registers using an 
+invalid email format</t>
+  </si>
+  <si>
+    <t>User registers with an email
+ that already exists in the system</t>
+  </si>
+  <si>
+    <t>User registers with a password
+ that does not meet requirements</t>
+  </si>
+  <si>
+    <t>Password and confirm password do 
+not match during registration</t>
+  </si>
+  <si>
+    <t>User enters invalid data (spaces) in 
+name field</t>
+  </si>
+  <si>
+    <t>User submits the register
+form with empty required fields</t>
+  </si>
+  <si>
+    <t>User registers an account 
+with all valid required  information</t>
   </si>
 </sst>
 </file>
@@ -370,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,11 +472,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="22">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -418,114 +509,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -602,6 +586,212 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -649,21 +839,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J8" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J8" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <autoFilter ref="A1:J8"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="TestCase ID" dataDxfId="9"/>
-    <tableColumn id="2" name="Title" dataDxfId="8"/>
-    <tableColumn id="3" name="Precondition" dataDxfId="7"/>
-    <tableColumn id="4" name="Priority" dataDxfId="6"/>
-    <tableColumn id="5" name="Test Steps" dataDxfId="5"/>
-    <tableColumn id="6" name="Test Data" dataDxfId="4"/>
-    <tableColumn id="7" name="Expected Result" dataDxfId="3"/>
-    <tableColumn id="8" name="Actual Result" dataDxfId="2"/>
-    <tableColumn id="9" name="Status" dataDxfId="1"/>
-    <tableColumn id="10" name="Note" dataDxfId="0"/>
+    <tableColumn id="1" name="TestCase ID" dataDxfId="17"/>
+    <tableColumn id="2" name="Title" dataDxfId="16"/>
+    <tableColumn id="3" name="Precondition" dataDxfId="15"/>
+    <tableColumn id="4" name="Priority" dataDxfId="14"/>
+    <tableColumn id="5" name="Test Steps" dataDxfId="13"/>
+    <tableColumn id="6" name="Test Data" dataDxfId="12"/>
+    <tableColumn id="7" name="Expected Result" dataDxfId="11"/>
+    <tableColumn id="8" name="Actual Result" dataDxfId="10"/>
+    <tableColumn id="9" name="Status" dataDxfId="9"/>
+    <tableColumn id="10" name="Note" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D8" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:D8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Scenario ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Scenario Name" dataDxfId="3"/>
+    <tableColumn id="3" name="Scenario Description" dataDxfId="2"/>
+    <tableColumn id="4" name="Related Test Case" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -932,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView zoomScale="48" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1169,4 +1372,140 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>